<commit_message>
Documentation for apoc.load.csv and apoc.load.xls
</commit_message>
<xml_diff>
--- a/src/test/resources/load_test.xlsx
+++ b/src/test/resources/load_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="9140" windowWidth="16020" windowHeight="5940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="780" yWindow="9140" windowWidth="16020" windowHeight="5940" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Full" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>